<commit_message>
User checkpoint: Refactor template rendering to use 'fieldname' instead of 'label'.  Remove unused emotion-cache related imports.
</commit_message>
<xml_diff>
--- a/uploads/Customer_template.xlsx
+++ b/uploads/Customer_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,92 +436,57 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Customer Name</t>
+          <t>customer_name [Data]</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Customer Type</t>
+          <t>customer_type [Select]</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Is Internal Customer</t>
+          <t>is_internal_customer [Check]</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Allowed To Transact With</t>
+          <t>website [Data]</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Website</t>
+          <t>customer_details [Text]</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Customer Details</t>
+          <t>tax_id [Data]</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Mobile No</t>
+          <t>default_commission_rate [Float]</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Email Id</t>
+          <t>so_required [Check]</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Tax ID</t>
+          <t>dn_required [Check]</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Credit Limit</t>
+          <t>is_frozen [Check]</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Accounts</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Sales Team</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Commission Rate</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Allow Sales Invoice Creation Without Sales Order</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Allow Sales Invoice Creation Without Delivery Note</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Is Frozen</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Disabled</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Customer Portal Users</t>
+          <t>disabled [Check]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
User checkpoint: Add @emotion/cache, @emotion/hash, and @emotion/is-prop-valid packages.
</commit_message>
<xml_diff>
--- a/uploads/Customer_template.xlsx
+++ b/uploads/Customer_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,26 @@
           <t>disabled [Check]</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>credit_limits.credit_limit [Currency]</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>credit_limits.bypass_credit_limit_check [Check]</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.allocated_percentage [Float]</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.incentives [Currency]</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
User checkpoint: Update Customer_template.xlsx
</commit_message>
<xml_diff>
--- a/uploads/Customer_template.xlsx
+++ b/uploads/Customer_template.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,47 +467,188 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>credit_limits.1.credit_limit [Currency]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>credit_limits.1.bypass_credit_limit_check [Check]</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>credit_limits.2.credit_limit [Currency]</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>credit_limits.2.bypass_credit_limit_check [Check]</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>credit_limits.3.credit_limit [Currency]</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>credit_limits.3.bypass_credit_limit_check [Check]</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>credit_limits.4.credit_limit [Currency]</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>credit_limits.4.bypass_credit_limit_check [Check]</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>credit_limits.5.credit_limit [Currency]</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>credit_limits.5.bypass_credit_limit_check [Check]</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.1.allocated_percentage [Float]</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.1.incentives [Currency]</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.2.allocated_percentage [Float]</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.2.incentives [Currency]</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.3.allocated_percentage [Float]</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.3.incentives [Currency]</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.4.allocated_percentage [Float]</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.4.incentives [Currency]</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.5.allocated_percentage [Float]</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>sales_team.5.incentives [Currency]</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
           <t>default_commission_rate [Float]</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>so_required [Check]</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>dn_required [Check]</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>is_frozen [Check]</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>disabled [Check]</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>credit_limits.credit_limit [Currency]</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>credit_limits.bypass_credit_limit_check [Check]</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>sales_team.allocated_percentage [Float]</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>sales_team.incentives [Currency]</t>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Instructions</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>For child tables:</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>- Each child table has 5 sets of columns</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>- Column format: tablename.row_number.fieldname</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>- Example: items.1.item_name, items.2.item_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>- Leave cells empty if not needed</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
User checkpoint: Update bundle.js; no changes to Customer_template.xlsx
</commit_message>
<xml_diff>
--- a/uploads/Customer_template.xlsx
+++ b/uploads/Customer_template.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:BA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,155 +437,265 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>salutation [Link]</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>customer_name [Data]</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>customer_type [Select]</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>customer_group [Link]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>territory [Link]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>gender [Link]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>lead_name [Link]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>opportunity_name [Link]</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>prospect_name [Link]</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>account_manager [Link]</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>default_currency [Link]</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>default_bank_account [Link]</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>default_price_list [Link]</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>is_internal_customer [Check]</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>represents_company [Link]</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>market_segment [Link]</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>industry [Link]</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>website [Data]</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>language [Link]</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>customer_details [Text]</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_address [Link]</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_contact [Link]</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>tax_id [Data]</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>tax_category [Link]</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>tax_withholding_category [Link]</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>payment_terms [Link]</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>credit_limits.1.credit_limit [Currency]</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>credit_limits.1.bypass_credit_limit_check [Check]</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>credit_limits.2.credit_limit [Currency]</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>credit_limits.2.bypass_credit_limit_check [Check]</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>credit_limits.3.credit_limit [Currency]</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>credit_limits.3.bypass_credit_limit_check [Check]</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>credit_limits.4.credit_limit [Currency]</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>credit_limits.4.bypass_credit_limit_check [Check]</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>credit_limits.5.credit_limit [Currency]</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>credit_limits.5.bypass_credit_limit_check [Check]</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>loyalty_program [Link]</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>sales_team.1.allocated_percentage [Float]</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>sales_team.1.incentives [Currency]</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>sales_team.2.allocated_percentage [Float]</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>sales_team.2.incentives [Currency]</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>sales_team.3.allocated_percentage [Float]</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>sales_team.3.incentives [Currency]</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>sales_team.4.allocated_percentage [Float]</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>sales_team.4.incentives [Currency]</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>sales_team.5.allocated_percentage [Float]</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>sales_team.5.incentives [Currency]</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>default_sales_partner [Link]</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>default_commission_rate [Float]</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>so_required [Check]</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>dn_required [Check]</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>is_frozen [Check]</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>disabled [Check]</t>
         </is>

</xml_diff>

<commit_message>
User checkpoint: Remove template instructions sheet from excel export.
</commit_message>
<xml_diff>
--- a/uploads/Customer_template.xlsx
+++ b/uploads/Customer_template.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Instructions" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -704,65 +703,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Instructions</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>For child tables:</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>- Each child table has 5 sets of columns</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>- Column format: tablename.row_number.fieldname</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>- Example: items.1.item_name, items.2.item_name</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>- Leave cells empty if not needed</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
User checkpoint: Improve handling of Link fields in template generation, including options.
</commit_message>
<xml_diff>
--- a/uploads/Customer_template.xlsx
+++ b/uploads/Customer_template.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>salutation [Link]</t>
+          <t>salutation [Link] [Salutation]</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -451,52 +451,52 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>customer_group [Link]</t>
+          <t>customer_group [Link] [Customer Group]</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>territory [Link]</t>
+          <t>territory [Link] [Territory]</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>gender [Link]</t>
+          <t>gender [Link] [Gender]</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>lead_name [Link]</t>
+          <t>lead_name [Link] [Lead]</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>opportunity_name [Link]</t>
+          <t>opportunity_name [Link] [Opportunity]</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>prospect_name [Link]</t>
+          <t>prospect_name [Link] [Prospect]</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>account_manager [Link]</t>
+          <t>account_manager [Link] [User]</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>default_currency [Link]</t>
+          <t>default_currency [Link] [Currency]</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>default_bank_account [Link]</t>
+          <t>default_bank_account [Link] [Bank Account]</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>default_price_list [Link]</t>
+          <t>default_price_list [Link] [Price List]</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -506,17 +506,17 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>represents_company [Link]</t>
+          <t>represents_company [Link] [Company]</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>market_segment [Link]</t>
+          <t>market_segment [Link] [Market Segment]</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>industry [Link]</t>
+          <t>industry [Link] [Industry Type]</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>language [Link]</t>
+          <t>language [Link] [Language]</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
@@ -536,12 +536,12 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>customer_primary_address [Link]</t>
+          <t>customer_primary_address [Link] [Address]</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>customer_primary_contact [Link]</t>
+          <t>customer_primary_contact [Link] [Contact]</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
@@ -551,17 +551,17 @@
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>tax_category [Link]</t>
+          <t>tax_category [Link] [Tax Category]</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>tax_withholding_category [Link]</t>
+          <t>tax_withholding_category [Link] [Tax Withholding Category]</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>payment_terms [Link]</t>
+          <t>payment_terms [Link] [Payment Terms Template]</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>loyalty_program [Link]</t>
+          <t>loyalty_program [Link] [Loyalty Program]</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>default_sales_partner [Link]</t>
+          <t>default_sales_partner [Link] [Sales Partner]</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">

</xml_diff>

<commit_message>
User checkpoint: Add customer data validation and importer method.
</commit_message>
<xml_diff>
--- a/uploads/Customer_template.xlsx
+++ b/uploads/Customer_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,37 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>customer_type [Select]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>customer_group [Link [Customer Group]]</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>territory [Link [Territory]]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>default_currency [Link [Currency]]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>default_price_list [Link [Price List]]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>tax_id [Data]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>payment_terms [Link [Payment Terms Template]]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
User checkpoint: Enhance customer template handler to include primary and secondary address fields.
</commit_message>
<xml_diff>
--- a/uploads/Customer_template.xlsx
+++ b/uploads/Customer_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,106 @@
           <t>payment_terms [Link [Payment Terms Template]]</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_address.address_title</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_address.address_line1</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_address.address_line2</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_address.city</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_address.state</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_address.zipcode</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_address.country</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_address.phone</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_address.email</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>customer_primary_address.address_type</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>customer_secondary_address.address_title</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>customer_secondary_address.address_line1</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>customer_secondary_address.address_line2</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>customer_secondary_address.city</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>customer_secondary_address.state</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>customer_secondary_address.zipcode</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>customer_secondary_address.country</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>customer_secondary_address.phone</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>customer_secondary_address.email</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>customer_secondary_address.address_type</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>